<commit_message>
adding Aspergillus niger SBMLs and updating Fungal_Models.xlsx
</commit_message>
<xml_diff>
--- a/Integration/Fungal_Models.xlsx
+++ b/Integration/Fungal_Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaver/Projects/ModelSEEDDatabase/Integration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jplfaria/repos/ModelSEEDDatabase/Integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EBDE092-EC3B-8F41-AF92-A473D74DE7C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9894D2-8296-4848-A2BC-1C2768DC11BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1080" windowWidth="37160" windowHeight="22440" xr2:uid="{21CDB662-67D8-4CA8-B684-CB4519F661E0}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="37160" windowHeight="19120" xr2:uid="{21CDB662-67D8-4CA8-B684-CB4519F661E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Fungal_Models" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
   <si>
     <t>iMM904</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>PLoS (SBML)</t>
+  </si>
+  <si>
+    <t>iJB1325</t>
+  </si>
+  <si>
+    <t>A community-driven reconstruction of the Aspergillus niger metabolic network.</t>
+  </si>
+  <si>
+    <t>Aspergillus niger ATCC 1015</t>
+  </si>
+  <si>
+    <t>Aspergillus niger CBS 513.88</t>
   </si>
 </sst>
 </file>
@@ -671,17 +683,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D46EC4-A80C-4D76-904D-ECD5CCB116FF}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="88.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
@@ -1080,8 +1092,48 @@
         <v>59</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="13">
+        <v>30275963</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="13">
+        <v>30275963</v>
+      </c>
+      <c r="C22" s="11">
+        <v>2018</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:F19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
     <sortCondition ref="C1"/>
   </sortState>
   <hyperlinks>
@@ -1122,6 +1174,10 @@
     <hyperlink ref="F18" r:id="rId35" xr:uid="{CC36898F-6A0D-3A41-B518-122D66EA3273}"/>
     <hyperlink ref="F19" r:id="rId36" xr:uid="{B0BAEBDD-B816-5543-8C50-2D1F9BB4996E}"/>
     <hyperlink ref="F20" r:id="rId37" xr:uid="{B28921F2-BDBB-184F-A66F-AB1EE22EFA4F}"/>
+    <hyperlink ref="B21" r:id="rId38" display="https://www.ncbi.nlm.nih.gov/pubmed/30275963" xr:uid="{28AF1510-45AD-4044-B923-CC84E461B10E}"/>
+    <hyperlink ref="B22" r:id="rId39" display="https://www.ncbi.nlm.nih.gov/pubmed/30275963" xr:uid="{592956B6-1EFA-9949-B324-D349D9FBF85D}"/>
+    <hyperlink ref="F21" r:id="rId40" xr:uid="{40CA0CF1-2FA5-B34E-B70D-A042F966AD05}"/>
+    <hyperlink ref="F22" r:id="rId41" xr:uid="{D7C623AB-0B07-0A4B-B1CF-725FCC9CBB4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>